<commit_message>
added FicsIt-Networks Api Documentation
</commit_message>
<xml_diff>
--- a/Ficsit-Documentation.xlsx
+++ b/Ficsit-Documentation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="86">
   <si>
     <t xml:space="preserve">filesystem</t>
   </si>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">[timeout:number]</t>
   </si>
   <si>
-    <t xml:space="preserve">file*</t>
+    <t xml:space="preserve">File</t>
   </si>
   <si>
     <t xml:space="preserve">open</t>
@@ -268,10 +268,7 @@
     <t xml:space="preserve">arg1:[int,]</t>
   </si>
   <si>
-    <t xml:space="preserve">arg2:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arg3:string</t>
+    <t xml:space="preserve">arg2:string …</t>
   </si>
   <si>
     <t xml:space="preserve">analyzePath</t>
@@ -387,8 +384,8 @@
   </sheetPr>
   <dimension ref="A2:AA24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V10" activeCellId="0" sqref="V10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,13 +393,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="22.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="1" width="22.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="7.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="25.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="17" style="1" width="22.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="7.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="25.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="24" style="1" width="22.98"/>
   </cols>
@@ -444,7 +441,7 @@
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -462,7 +459,7 @@
       <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="P3" s="1" t="s">
@@ -480,7 +477,7 @@
       <c r="T3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="V3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="W3" s="1" t="s">
@@ -515,7 +512,7 @@
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -524,7 +521,7 @@
       <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="O5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="1" t="s">
@@ -536,7 +533,7 @@
       <c r="R5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="0" t="s">
+      <c r="V5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="W5" s="1" t="s">
@@ -562,7 +559,7 @@
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -571,7 +568,7 @@
       <c r="J6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="O6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="P6" s="1" t="s">
@@ -583,7 +580,7 @@
       <c r="R6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V6" s="0" t="s">
+      <c r="V6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="W6" s="1" t="s">
@@ -606,7 +603,7 @@
       <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -615,7 +612,7 @@
       <c r="J7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="V7" s="0" t="s">
+      <c r="V7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="W7" s="1" t="s">
@@ -644,7 +641,7 @@
       <c r="E8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -656,7 +653,7 @@
       <c r="K8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V8" s="0" t="s">
+      <c r="V8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="W8" s="1" t="s">
@@ -682,7 +679,7 @@
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -691,7 +688,7 @@
       <c r="J9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="V9" s="0" t="s">
+      <c r="V9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="W9" s="1" t="s">
@@ -714,7 +711,7 @@
       <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -723,7 +720,7 @@
       <c r="J10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V10" s="0" t="s">
+      <c r="V10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="W10" s="1" t="s">
@@ -749,7 +746,7 @@
       <c r="E11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -775,7 +772,7 @@
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -798,7 +795,7 @@
       <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -821,7 +818,7 @@
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -847,7 +844,7 @@
       <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -870,7 +867,7 @@
       <c r="D16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -893,7 +890,7 @@
       <c r="D17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -919,7 +916,7 @@
       <c r="E18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -942,7 +939,7 @@
       <c r="D19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -996,9 +993,6 @@
       <c r="E22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -1008,10 +1002,10 @@
         <v>54</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,10 +1016,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1033,8 +1027,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>